<commit_message>
conditional formatting added to .xlsx sheet to strikethrough patients with only one scan
</commit_message>
<xml_diff>
--- a/patient_timeline_map.xlsx
+++ b/patient_timeline_map.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottebrass/repos/FSL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18E04DC9-9BEB-D347-86FB-646D1E8DD40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54F0933A-7DE1-6043-B791-FB8D1673664C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{4D4E7ECD-C86E-C045-AF47-2EDB634FD938}"/>
   </bookViews>
   <sheets>
     <sheet name="hemi" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
   <si>
     <t>Patient ID</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>Inclusion comments</t>
+  </si>
+  <si>
+    <t>fluid build up instead of brain expansion</t>
+  </si>
+  <si>
+    <t>ventricle enlargement (ventriculomegaly // hydrocephalus)</t>
+  </si>
+  <si>
+    <t>acute yes, fast ?? Skull edges difficult (skull edges always difficult)</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
 </sst>
 </file>
@@ -104,16 +119,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -127,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -167,7 +204,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -273,7 +310,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -415,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -423,19 +460,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B49229-670B-CC40-8F91-AF62019E1911}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="8" width="10.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +501,14 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12519</v>
       </c>
@@ -483,8 +527,15 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="1">
+        <f>SUM(B2:H2)</f>
+        <v>4</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13198</v>
       </c>
@@ -500,8 +551,15 @@
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J34" si="0">SUM(B3:H3)</f>
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13294</v>
       </c>
@@ -511,8 +569,15 @@
       <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13318</v>
       </c>
@@ -522,8 +587,15 @@
       <c r="I5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>13782</v>
       </c>
@@ -536,8 +608,12 @@
       <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>13990</v>
       </c>
@@ -550,8 +626,12 @@
       <c r="I7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>14324</v>
       </c>
@@ -567,8 +647,12 @@
       <c r="I8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16577</v>
       </c>
@@ -578,8 +662,12 @@
       <c r="I9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16754</v>
       </c>
@@ -592,8 +680,12 @@
       <c r="I10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>17746</v>
       </c>
@@ -603,8 +695,12 @@
       <c r="I11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>19344</v>
       </c>
@@ -617,8 +713,12 @@
       <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>19575</v>
       </c>
@@ -631,8 +731,12 @@
       <c r="I13" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>19978</v>
       </c>
@@ -648,8 +752,12 @@
       <c r="I14" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>19981</v>
       </c>
@@ -665,8 +773,12 @@
       <c r="I15" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20174</v>
       </c>
@@ -685,8 +797,12 @@
       <c r="I16" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20651</v>
       </c>
@@ -699,8 +815,12 @@
       <c r="I17" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20809</v>
       </c>
@@ -710,8 +830,12 @@
       <c r="I18" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20942</v>
       </c>
@@ -730,8 +854,12 @@
       <c r="I19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>21221</v>
       </c>
@@ -744,8 +872,12 @@
       <c r="I20" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21390</v>
       </c>
@@ -755,8 +887,12 @@
       <c r="I21" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21494</v>
       </c>
@@ -766,8 +902,12 @@
       <c r="I22" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22725</v>
       </c>
@@ -783,8 +923,12 @@
       <c r="I23" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22785</v>
       </c>
@@ -800,8 +944,12 @@
       <c r="I24" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23348</v>
       </c>
@@ -814,8 +962,12 @@
       <c r="I25" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23355</v>
       </c>
@@ -825,8 +977,12 @@
       <c r="I26" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>12294</v>
       </c>
@@ -839,8 +995,12 @@
       <c r="I28" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>12356</v>
       </c>
@@ -862,8 +1022,12 @@
       <c r="I29" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>13971</v>
       </c>
@@ -879,8 +1043,12 @@
       <c r="I30" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>17813</v>
       </c>
@@ -893,8 +1061,12 @@
       <c r="I31" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>17980</v>
       </c>
@@ -910,8 +1082,12 @@
       <c r="I32" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20135</v>
       </c>
@@ -927,8 +1103,12 @@
       <c r="I33" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>21720</v>
       </c>
@@ -938,8 +1118,17 @@
       <c r="I34" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="J34" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:I34">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>SUM($B2:$H2)&lt;2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved comments to correct line
</commit_message>
<xml_diff>
--- a/patient_timeline_map.xlsx
+++ b/patient_timeline_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottebrass/repos/FSL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EBACEB-DB74-1441-B0D2-449F1386E6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EB20F0-014A-1F4B-9B1A-8691E2AD79DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4D4E7ECD-C86E-C045-AF47-2EDB634FD938}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,9 +554,6 @@
       <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K4" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -568,9 +565,6 @@
       <c r="I5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -585,6 +579,9 @@
       <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -598,6 +595,9 @@
       </c>
       <c r="I7" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added comments to hemi patients
</commit_message>
<xml_diff>
--- a/patient_timeline_map.xlsx
+++ b/patient_timeline_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottebrass/repos/FSL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EB20F0-014A-1F4B-9B1A-8691E2AD79DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F967D3C-628C-7842-9D7E-66A379B63C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4D4E7ECD-C86E-C045-AF47-2EDB634FD938}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>Patient ID</t>
   </si>
@@ -81,14 +81,70 @@
   </si>
   <si>
     <t>acute yes, fast ?? Skull edges difficult (skull edges always difficult)</t>
+  </si>
+  <si>
+    <t>Inclusion?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Skull can easily be seen, non symmetrical expansion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interesting compression - the skin follows shape of symmetrical expansion but lesion is pressing on expansion as well. </t>
+  </si>
+  <si>
+    <t>Skull visible, mostly symmetrical expansion considering nothing is spherical</t>
+  </si>
+  <si>
+    <t>Not much expansion</t>
+  </si>
+  <si>
+    <t>hard to see skull anchor points but makes a very nice shape, little else confounding the image</t>
+  </si>
+  <si>
+    <t>like 12519, fluid build up instead of brain expansion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ultra-fast to fast only - acute is wildly deformed. 3 months is okay. </t>
+  </si>
+  <si>
+    <t>lesion layer on top of free bulge</t>
+  </si>
+  <si>
+    <t>non symmetrical expansion, easy to see skull points</t>
+  </si>
+  <si>
+    <t>brain didn’t change shape sufficiently</t>
+  </si>
+  <si>
+    <t>!! THE BEST ONE</t>
+  </si>
+  <si>
+    <t>could be good - bad registration</t>
+  </si>
+  <si>
+    <t>??tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">push back on expansion in sigmoid shape -&gt; fills out over time. 3 months = ventriculomegaly </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -116,13 +172,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,19 +516,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B49229-670B-CC40-8F91-AF62019E1911}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="8" width="10.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,11 +557,14 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12519</v>
       </c>
@@ -520,11 +583,11 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13198</v>
       </c>
@@ -540,11 +603,11 @@
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13294</v>
       </c>
@@ -555,7 +618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13318</v>
       </c>
@@ -566,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>13782</v>
       </c>
@@ -579,11 +642,11 @@
       <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>13990</v>
       </c>
@@ -596,11 +659,14 @@
       <c r="I7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>14324</v>
       </c>
@@ -616,8 +682,14 @@
       <c r="I8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16577</v>
       </c>
@@ -628,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16754</v>
       </c>
@@ -641,8 +713,14 @@
       <c r="I10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>17746</v>
       </c>
@@ -653,7 +731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>19344</v>
       </c>
@@ -666,8 +744,14 @@
       <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>19575</v>
       </c>
@@ -680,8 +764,11 @@
       <c r="I13" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>19978</v>
       </c>
@@ -697,8 +784,14 @@
       <c r="I14" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>19981</v>
       </c>
@@ -714,8 +807,11 @@
       <c r="I15" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20174</v>
       </c>
@@ -734,8 +830,14 @@
       <c r="I16" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20651</v>
       </c>
@@ -748,8 +850,11 @@
       <c r="I17" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20809</v>
       </c>
@@ -760,7 +865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20942</v>
       </c>
@@ -779,8 +884,14 @@
       <c r="I19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>21221</v>
       </c>
@@ -793,8 +904,11 @@
       <c r="I20" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21390</v>
       </c>
@@ -805,7 +919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21494</v>
       </c>
@@ -816,7 +930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22725</v>
       </c>
@@ -832,8 +946,14 @@
       <c r="I23" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22785</v>
       </c>
@@ -849,8 +969,14 @@
       <c r="I24" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23348</v>
       </c>
@@ -863,8 +989,11 @@
       <c r="I25" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23355</v>
       </c>
@@ -875,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>12294</v>
       </c>
@@ -889,7 +1018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>12356</v>
       </c>
@@ -912,7 +1041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>13971</v>
       </c>
@@ -929,7 +1058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>17813</v>
       </c>
@@ -943,7 +1072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>17980</v>
       </c>

</xml_diff>